<commit_message>
move row that removes clientUpdateProhibited so subsequent tests don't fail
</commit_message>
<xml_diff>
--- a/data/epp-13-status-data.xlsx
+++ b/data/epp-13-status-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B5CE9C-AFAC-8545-B559-1D5143641C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1885A050-A6E4-6641-9833-202F3F8BB054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="30">
   <si>
     <t>errorCode</t>
   </si>
@@ -737,7 +737,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,16 +842,10 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -859,13 +853,13 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -873,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -887,7 +881,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -901,7 +895,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -915,7 +909,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -929,7 +923,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -943,7 +937,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -957,7 +951,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -971,7 +965,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
@@ -985,7 +979,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1</v>
@@ -996,16 +990,16 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>